<commit_message>
expanded section 5-2a graphs
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="204">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -2037,7 +2037,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2045,7 +2045,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -2125,19 +2125,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -2332,11 +2332,11 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A314" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C330" activeCellId="0" sqref="C330"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A161" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D179" activeCellId="0" sqref="D179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
@@ -5093,19 +5093,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="104" t="s">
         <v>84</v>
       </c>
-      <c r="C178" s="105"/>
-      <c r="D178" s="106"/>
-      <c r="E178" s="68"/>
-      <c r="F178" s="106"/>
-      <c r="G178" s="106"/>
-      <c r="H178" s="107"/>
-      <c r="I178" s="68"/>
-      <c r="J178" s="106"/>
-      <c r="K178" s="108"/>
+      <c r="C178" s="105" t="n">
+        <v>-2.02</v>
+      </c>
+      <c r="D178" s="106" t="n">
+        <v>-37.98</v>
+      </c>
+      <c r="E178" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="F178" s="106" t="n">
+        <v>31</v>
+      </c>
+      <c r="G178" s="106" t="n">
+        <v>24</v>
+      </c>
+      <c r="H178" s="107" t="n">
+        <v>24.73</v>
+      </c>
+      <c r="I178" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="J178" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="K178" s="108" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E179" s="13" t="s">

</xml_diff>

<commit_message>
added free float temperature table, and general graphics, added.
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="204">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -2332,11 +2332,11 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A161" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D179" activeCellId="0" sqref="D179"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C130" activeCellId="0" sqref="C130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
@@ -4750,99 +4750,225 @@
       <c r="B130" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C130" s="80"/>
-      <c r="D130" s="54"/>
-      <c r="E130" s="56"/>
-      <c r="F130" s="81"/>
-      <c r="G130" s="81"/>
-      <c r="H130" s="82"/>
-      <c r="I130" s="56"/>
-      <c r="J130" s="81"/>
-      <c r="K130" s="58"/>
+      <c r="C130" s="80" t="n">
+        <v>24.92</v>
+      </c>
+      <c r="D130" s="54" t="n">
+        <v>-12.56</v>
+      </c>
+      <c r="E130" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F130" s="81" t="n">
+        <v>9</v>
+      </c>
+      <c r="G130" s="81" t="n">
+        <v>7</v>
+      </c>
+      <c r="H130" s="82" t="n">
+        <v>63.84</v>
+      </c>
+      <c r="I130" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="J130" s="81" t="n">
+        <v>18</v>
+      </c>
+      <c r="K130" s="58" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="C131" s="83"/>
-      <c r="D131" s="59"/>
-      <c r="E131" s="56"/>
-      <c r="F131" s="56"/>
-      <c r="G131" s="56"/>
-      <c r="H131" s="57"/>
-      <c r="I131" s="56"/>
-      <c r="J131" s="56"/>
-      <c r="K131" s="62"/>
+      <c r="C131" s="83" t="n">
+        <v>25.12</v>
+      </c>
+      <c r="D131" s="59" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E131" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F131" s="56" t="n">
+        <v>9</v>
+      </c>
+      <c r="G131" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="H131" s="57" t="n">
+        <v>44.29</v>
+      </c>
+      <c r="I131" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="J131" s="56" t="n">
+        <v>12</v>
+      </c>
+      <c r="K131" s="62" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="C132" s="83"/>
-      <c r="D132" s="59"/>
-      <c r="E132" s="56"/>
-      <c r="F132" s="56"/>
-      <c r="G132" s="56"/>
-      <c r="H132" s="57"/>
-      <c r="I132" s="56"/>
-      <c r="J132" s="56"/>
-      <c r="K132" s="62"/>
+      <c r="C132" s="83" t="n">
+        <v>18.42</v>
+      </c>
+      <c r="D132" s="59" t="n">
+        <v>-17.08</v>
+      </c>
+      <c r="E132" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F132" s="56" t="n">
+        <v>31</v>
+      </c>
+      <c r="G132" s="56" t="n">
+        <v>24</v>
+      </c>
+      <c r="H132" s="57" t="n">
+        <v>62.47</v>
+      </c>
+      <c r="I132" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="J132" s="56" t="n">
+        <v>18</v>
+      </c>
+      <c r="K132" s="62" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="C133" s="83"/>
-      <c r="D133" s="59"/>
-      <c r="E133" s="56"/>
-      <c r="F133" s="56"/>
-      <c r="G133" s="56"/>
-      <c r="H133" s="57"/>
-      <c r="I133" s="56"/>
-      <c r="J133" s="56"/>
-      <c r="K133" s="62"/>
+      <c r="C133" s="83" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="D133" s="59" t="n">
+        <v>-12.81</v>
+      </c>
+      <c r="E133" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F133" s="56" t="n">
+        <v>9</v>
+      </c>
+      <c r="G133" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="H133" s="57" t="n">
+        <v>36.68</v>
+      </c>
+      <c r="I133" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="J133" s="56" t="n">
+        <v>11</v>
+      </c>
+      <c r="K133" s="62" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="C134" s="83"/>
-      <c r="D134" s="59"/>
-      <c r="E134" s="56"/>
-      <c r="F134" s="56"/>
-      <c r="G134" s="56"/>
-      <c r="H134" s="57"/>
-      <c r="I134" s="56"/>
-      <c r="J134" s="56"/>
-      <c r="K134" s="62"/>
+      <c r="C134" s="83" t="n">
+        <v>30.96</v>
+      </c>
+      <c r="D134" s="59" t="n">
+        <v>-7.05</v>
+      </c>
+      <c r="E134" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F134" s="56" t="n">
+        <v>9</v>
+      </c>
+      <c r="G134" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="H134" s="57" t="n">
+        <v>70.14</v>
+      </c>
+      <c r="I134" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="J134" s="56" t="n">
+        <v>22</v>
+      </c>
+      <c r="K134" s="62" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="C135" s="83"/>
-      <c r="D135" s="59"/>
-      <c r="E135" s="56"/>
-      <c r="F135" s="56"/>
-      <c r="G135" s="56"/>
-      <c r="H135" s="57"/>
-      <c r="I135" s="56"/>
-      <c r="J135" s="56"/>
-      <c r="K135" s="62"/>
+      <c r="C135" s="83" t="n">
+        <v>31.16</v>
+      </c>
+      <c r="D135" s="59" t="n">
+        <v>9.92</v>
+      </c>
+      <c r="E135" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="F135" s="56" t="n">
+        <v>4</v>
+      </c>
+      <c r="G135" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="H135" s="57" t="n">
+        <v>49.62</v>
+      </c>
+      <c r="I135" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="J135" s="56" t="n">
+        <v>12</v>
+      </c>
+      <c r="K135" s="62" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="C136" s="85"/>
-      <c r="D136" s="66"/>
-      <c r="E136" s="68"/>
-      <c r="F136" s="68"/>
-      <c r="G136" s="68"/>
-      <c r="H136" s="86"/>
-      <c r="I136" s="68"/>
-      <c r="J136" s="68"/>
-      <c r="K136" s="70"/>
+      <c r="C136" s="85" t="n">
+        <v>27.74</v>
+      </c>
+      <c r="D136" s="66" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="E136" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="F136" s="68" t="n">
+        <v>9</v>
+      </c>
+      <c r="G136" s="68" t="n">
+        <v>7</v>
+      </c>
+      <c r="H136" s="86" t="n">
+        <v>49.88</v>
+      </c>
+      <c r="I136" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="J136" s="68" t="n">
+        <v>12</v>
+      </c>
+      <c r="K136" s="70" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E137" s="13" t="s">

</xml_diff>

<commit_message>
flake8 fixes and testing github workflow on new branch
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -427,7 +427,7 @@
     <t xml:space="preserve">Software:</t>
   </si>
   <si>
-    <t xml:space="preserve">TestSoftware</t>
+    <t xml:space="preserve">TestSoftwareProgram</t>
   </si>
   <si>
     <t xml:space="preserve">Version:</t>
@@ -2336,7 +2336,7 @@
       <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>

</xml_diff>

<commit_message>
added individual graphic rendering option and processing
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -427,7 +427,7 @@
     <t xml:space="preserve">Software:</t>
   </si>
   <si>
-    <t xml:space="preserve">TestSoftware11111</t>
+    <t xml:space="preserve">TestSoftware</t>
   </si>
   <si>
     <t xml:space="preserve">Version:</t>
@@ -2336,7 +2336,7 @@
       <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>

</xml_diff>

<commit_message>
fix excel processor and image creation
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -427,7 +427,7 @@
     <t xml:space="preserve">Software:</t>
   </si>
   <si>
-    <t xml:space="preserve">TestSoftwareProgram</t>
+    <t xml:space="preserve">TestSoftware</t>
   </si>
   <si>
     <t xml:space="preserve">Version:</t>
@@ -2336,7 +2336,7 @@
       <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>

</xml_diff>

<commit_message>
added specific day hourly output free float zone temperature table
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -2344,11 +2344,11 @@
   </sheetPr>
   <dimension ref="A3:AO579"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B230" activeCellId="0" sqref="B230"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A288" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B294" activeCellId="0" sqref="B294"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="8" style="0" width="10.53"/>
@@ -9023,268 +9023,556 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B294" s="153" t="n">
+      <c r="B294" s="142" t="n">
         <v>1</v>
       </c>
-      <c r="C294" s="59"/>
-      <c r="D294" s="61"/>
-      <c r="E294" s="56"/>
-      <c r="F294" s="56"/>
-      <c r="G294" s="57"/>
-      <c r="H294" s="62"/>
+      <c r="C294" s="59" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="D294" s="61" t="n">
+        <v>12.94</v>
+      </c>
+      <c r="E294" s="56" t="n">
+        <v>19.87</v>
+      </c>
+      <c r="F294" s="56" t="n">
+        <v>21.23</v>
+      </c>
+      <c r="G294" s="57" t="n">
+        <v>15.35</v>
+      </c>
+      <c r="H294" s="62" t="n">
+        <v>22.75</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B295" s="157" t="n">
+      <c r="B295" s="143" t="n">
         <v>2</v>
       </c>
-      <c r="C295" s="59"/>
-      <c r="D295" s="61"/>
-      <c r="E295" s="56"/>
-      <c r="F295" s="56"/>
-      <c r="G295" s="57"/>
-      <c r="H295" s="62"/>
+      <c r="C295" s="59" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="D295" s="61" t="n">
+        <v>12.43</v>
+      </c>
+      <c r="E295" s="56" t="n">
+        <v>19.06</v>
+      </c>
+      <c r="F295" s="56" t="n">
+        <v>20.72</v>
+      </c>
+      <c r="G295" s="57" t="n">
+        <v>13.48</v>
+      </c>
+      <c r="H295" s="62" t="n">
+        <v>22.24</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B296" s="157" t="n">
+      <c r="B296" s="143" t="n">
         <v>3</v>
       </c>
-      <c r="C296" s="59"/>
-      <c r="D296" s="61"/>
-      <c r="E296" s="56"/>
-      <c r="F296" s="56"/>
-      <c r="G296" s="57"/>
-      <c r="H296" s="62"/>
+      <c r="C296" s="59" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="D296" s="61" t="n">
+        <v>11.93</v>
+      </c>
+      <c r="E296" s="56" t="n">
+        <v>18.14</v>
+      </c>
+      <c r="F296" s="56" t="n">
+        <v>20.03</v>
+      </c>
+      <c r="G296" s="57" t="n">
+        <v>11.78</v>
+      </c>
+      <c r="H296" s="62" t="n">
+        <v>21.76</v>
+      </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B297" s="157" t="n">
+      <c r="B297" s="143" t="n">
         <v>4</v>
       </c>
-      <c r="C297" s="59"/>
-      <c r="D297" s="61"/>
-      <c r="E297" s="56"/>
-      <c r="F297" s="56"/>
-      <c r="G297" s="57"/>
-      <c r="H297" s="62"/>
+      <c r="C297" s="59" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="D297" s="61" t="n">
+        <v>11.43</v>
+      </c>
+      <c r="E297" s="56" t="n">
+        <v>17.02</v>
+      </c>
+      <c r="F297" s="56" t="n">
+        <v>19.16</v>
+      </c>
+      <c r="G297" s="57" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="H297" s="62" t="n">
+        <v>21.28</v>
+      </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B298" s="157" t="n">
+      <c r="B298" s="143" t="n">
         <v>5</v>
       </c>
-      <c r="C298" s="59"/>
-      <c r="D298" s="61"/>
-      <c r="E298" s="56"/>
-      <c r="F298" s="56"/>
-      <c r="G298" s="57"/>
-      <c r="H298" s="62"/>
+      <c r="C298" s="59" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D298" s="61" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="E298" s="56" t="n">
+        <v>15.88</v>
+      </c>
+      <c r="F298" s="56" t="n">
+        <v>18.25</v>
+      </c>
+      <c r="G298" s="57" t="n">
+        <v>8.78</v>
+      </c>
+      <c r="H298" s="62" t="n">
+        <v>20.86</v>
+      </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B299" s="157" t="n">
+      <c r="B299" s="143" t="n">
         <v>6</v>
       </c>
-      <c r="C299" s="59"/>
-      <c r="D299" s="61"/>
-      <c r="E299" s="56"/>
-      <c r="F299" s="56"/>
-      <c r="G299" s="57"/>
-      <c r="H299" s="62"/>
+      <c r="C299" s="59" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="D299" s="61" t="n">
+        <v>10.58</v>
+      </c>
+      <c r="E299" s="56" t="n">
+        <v>16.39</v>
+      </c>
+      <c r="F299" s="56" t="n">
+        <v>18.63</v>
+      </c>
+      <c r="G299" s="57" t="n">
+        <v>7.51</v>
+      </c>
+      <c r="H299" s="62" t="n">
+        <v>20.46</v>
+      </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B300" s="157" t="n">
+      <c r="B300" s="143" t="n">
         <v>7</v>
       </c>
-      <c r="C300" s="59"/>
-      <c r="D300" s="61"/>
-      <c r="E300" s="56"/>
-      <c r="F300" s="56"/>
-      <c r="G300" s="57"/>
-      <c r="H300" s="62"/>
+      <c r="C300" s="59" t="n">
+        <v>-1.71</v>
+      </c>
+      <c r="D300" s="61" t="n">
+        <v>10.17</v>
+      </c>
+      <c r="E300" s="56" t="n">
+        <v>18.76</v>
+      </c>
+      <c r="F300" s="56" t="n">
+        <v>20.27</v>
+      </c>
+      <c r="G300" s="57" t="n">
+        <v>6.35</v>
+      </c>
+      <c r="H300" s="62" t="n">
+        <v>20.08</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B301" s="157" t="n">
+      <c r="B301" s="143" t="n">
         <v>8</v>
       </c>
-      <c r="C301" s="59"/>
-      <c r="D301" s="61"/>
-      <c r="E301" s="56"/>
-      <c r="F301" s="56"/>
-      <c r="G301" s="57"/>
-      <c r="H301" s="62"/>
+      <c r="C301" s="59" t="n">
+        <v>-1.48</v>
+      </c>
+      <c r="D301" s="61" t="n">
+        <v>10.32</v>
+      </c>
+      <c r="E301" s="56" t="n">
+        <v>20.89</v>
+      </c>
+      <c r="F301" s="56" t="n">
+        <v>22.87</v>
+      </c>
+      <c r="G301" s="57" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="H301" s="62" t="n">
+        <v>20.25</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B302" s="157" t="n">
+      <c r="B302" s="143" t="n">
         <v>9</v>
       </c>
-      <c r="C302" s="59"/>
-      <c r="D302" s="61"/>
-      <c r="E302" s="56"/>
-      <c r="F302" s="56"/>
-      <c r="G302" s="57"/>
-      <c r="H302" s="62"/>
+      <c r="C302" s="59" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="D302" s="61" t="n">
+        <v>11.75</v>
+      </c>
+      <c r="E302" s="56" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="F302" s="56" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="G302" s="57" t="n">
+        <v>10.04</v>
+      </c>
+      <c r="H302" s="62" t="n">
+        <v>21.66</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B303" s="157" t="n">
+      <c r="B303" s="143" t="n">
         <v>10</v>
       </c>
-      <c r="C303" s="59"/>
-      <c r="D303" s="61"/>
-      <c r="E303" s="56"/>
-      <c r="F303" s="56"/>
-      <c r="G303" s="57"/>
-      <c r="H303" s="62"/>
+      <c r="C303" s="59" t="n">
+        <v>9.93</v>
+      </c>
+      <c r="D303" s="61" t="n">
+        <v>13.81</v>
+      </c>
+      <c r="E303" s="56" t="n">
+        <v>26.43</v>
+      </c>
+      <c r="F303" s="56" t="n">
+        <v>25.57</v>
+      </c>
+      <c r="G303" s="57" t="n">
+        <v>16.59</v>
+      </c>
+      <c r="H303" s="62" t="n">
+        <v>23.55</v>
+      </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B304" s="157" t="n">
+      <c r="B304" s="143" t="n">
         <v>11</v>
       </c>
-      <c r="C304" s="59"/>
-      <c r="D304" s="61"/>
-      <c r="E304" s="56"/>
-      <c r="F304" s="56"/>
-      <c r="G304" s="57"/>
-      <c r="H304" s="62"/>
+      <c r="C304" s="59" t="n">
+        <v>18.73</v>
+      </c>
+      <c r="D304" s="61" t="n">
+        <v>15.96</v>
+      </c>
+      <c r="E304" s="56" t="n">
+        <v>30.62</v>
+      </c>
+      <c r="F304" s="56" t="n">
+        <v>26.91</v>
+      </c>
+      <c r="G304" s="57" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="H304" s="62" t="n">
+        <v>25.59</v>
+      </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B305" s="157" t="n">
+      <c r="B305" s="143" t="n">
         <v>12</v>
       </c>
-      <c r="C305" s="59"/>
-      <c r="D305" s="61"/>
-      <c r="E305" s="56"/>
-      <c r="F305" s="56"/>
-      <c r="G305" s="57"/>
-      <c r="H305" s="62"/>
+      <c r="C305" s="59" t="n">
+        <v>28.01</v>
+      </c>
+      <c r="D305" s="61" t="n">
+        <v>18.21</v>
+      </c>
+      <c r="E305" s="56" t="n">
+        <v>35.22</v>
+      </c>
+      <c r="F305" s="56" t="n">
+        <v>28.18</v>
+      </c>
+      <c r="G305" s="57" t="n">
+        <v>33.65</v>
+      </c>
+      <c r="H305" s="62" t="n">
+        <v>27.79</v>
+      </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B306" s="157" t="n">
+      <c r="B306" s="143" t="n">
         <v>13</v>
       </c>
-      <c r="C306" s="59"/>
-      <c r="D306" s="61"/>
-      <c r="E306" s="56"/>
-      <c r="F306" s="56"/>
-      <c r="G306" s="57"/>
-      <c r="H306" s="62"/>
+      <c r="C306" s="59" t="n">
+        <v>36.57</v>
+      </c>
+      <c r="D306" s="61" t="n">
+        <v>20.44</v>
+      </c>
+      <c r="E306" s="56" t="n">
+        <v>39.19</v>
+      </c>
+      <c r="F306" s="56" t="n">
+        <v>29.13</v>
+      </c>
+      <c r="G306" s="57" t="n">
+        <v>42.51</v>
+      </c>
+      <c r="H306" s="62" t="n">
+        <v>29.97</v>
+      </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B307" s="157" t="n">
+      <c r="B307" s="143" t="n">
         <v>14</v>
       </c>
-      <c r="C307" s="59"/>
-      <c r="D307" s="61"/>
-      <c r="E307" s="56"/>
-      <c r="F307" s="56"/>
-      <c r="G307" s="57"/>
-      <c r="H307" s="62"/>
+      <c r="C307" s="59" t="n">
+        <v>43.39</v>
+      </c>
+      <c r="D307" s="61" t="n">
+        <v>22.01</v>
+      </c>
+      <c r="E307" s="56" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="F307" s="56" t="n">
+        <v>29.86</v>
+      </c>
+      <c r="G307" s="57" t="n">
+        <v>49.77</v>
+      </c>
+      <c r="H307" s="62" t="n">
+        <v>31.47</v>
+      </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B308" s="157" t="n">
+      <c r="B308" s="143" t="n">
         <v>15</v>
       </c>
-      <c r="C308" s="59"/>
-      <c r="D308" s="61"/>
-      <c r="E308" s="56"/>
-      <c r="F308" s="56"/>
-      <c r="G308" s="57"/>
-      <c r="H308" s="62"/>
+      <c r="C308" s="59" t="n">
+        <v>46.98</v>
+      </c>
+      <c r="D308" s="61" t="n">
+        <v>22.72</v>
+      </c>
+      <c r="E308" s="56" t="n">
+        <v>44.21</v>
+      </c>
+      <c r="F308" s="56" t="n">
+        <v>30.29</v>
+      </c>
+      <c r="G308" s="57" t="n">
+        <v>54.39</v>
+      </c>
+      <c r="H308" s="62" t="n">
+        <v>32.08</v>
+      </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B309" s="157" t="n">
+      <c r="B309" s="143" t="n">
         <v>16</v>
       </c>
-      <c r="C309" s="59"/>
-      <c r="D309" s="61"/>
-      <c r="E309" s="56"/>
-      <c r="F309" s="56"/>
-      <c r="G309" s="57"/>
-      <c r="H309" s="62"/>
+      <c r="C309" s="59" t="n">
+        <v>47.59</v>
+      </c>
+      <c r="D309" s="61" t="n">
+        <v>22.82</v>
+      </c>
+      <c r="E309" s="56" t="n">
+        <v>44.89</v>
+      </c>
+      <c r="F309" s="56" t="n">
+        <v>30.43</v>
+      </c>
+      <c r="G309" s="57" t="n">
+        <v>56.31</v>
+      </c>
+      <c r="H309" s="62" t="n">
+        <v>32.2</v>
+      </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B310" s="157" t="n">
+      <c r="B310" s="143" t="n">
         <v>17</v>
       </c>
-      <c r="C310" s="59"/>
-      <c r="D310" s="61"/>
-      <c r="E310" s="56"/>
-      <c r="F310" s="56"/>
-      <c r="G310" s="57"/>
-      <c r="H310" s="62"/>
+      <c r="C310" s="59" t="n">
+        <v>44.88</v>
+      </c>
+      <c r="D310" s="61" t="n">
+        <v>22.1</v>
+      </c>
+      <c r="E310" s="56" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="F310" s="56" t="n">
+        <v>30.43</v>
+      </c>
+      <c r="G310" s="57" t="n">
+        <v>54.98</v>
+      </c>
+      <c r="H310" s="62" t="n">
+        <v>31.46</v>
+      </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B311" s="157" t="n">
+      <c r="B311" s="143" t="n">
         <v>18</v>
       </c>
-      <c r="C311" s="59"/>
-      <c r="D311" s="61"/>
-      <c r="E311" s="56"/>
-      <c r="F311" s="56"/>
-      <c r="G311" s="57"/>
-      <c r="H311" s="62"/>
+      <c r="C311" s="59" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="D311" s="61" t="n">
+        <v>20.49</v>
+      </c>
+      <c r="E311" s="56" t="n">
+        <v>43.74</v>
+      </c>
+      <c r="F311" s="56" t="n">
+        <v>30.35</v>
+      </c>
+      <c r="G311" s="57" t="n">
+        <v>50.21</v>
+      </c>
+      <c r="H311" s="62" t="n">
+        <v>29.83</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B312" s="157" t="n">
+      <c r="B312" s="143" t="n">
         <v>19</v>
       </c>
-      <c r="C312" s="59"/>
-      <c r="D312" s="61"/>
-      <c r="E312" s="56"/>
-      <c r="F312" s="56"/>
-      <c r="G312" s="57"/>
-      <c r="H312" s="62"/>
+      <c r="C312" s="59" t="n">
+        <v>32.16</v>
+      </c>
+      <c r="D312" s="61" t="n">
+        <v>19.22</v>
+      </c>
+      <c r="E312" s="56" t="n">
+        <v>34.48</v>
+      </c>
+      <c r="F312" s="56" t="n">
+        <v>29.03</v>
+      </c>
+      <c r="G312" s="57" t="n">
+        <v>44.93</v>
+      </c>
+      <c r="H312" s="62" t="n">
+        <v>28.67</v>
+      </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B313" s="157" t="n">
+      <c r="B313" s="143" t="n">
         <v>20</v>
       </c>
-      <c r="C313" s="59"/>
-      <c r="D313" s="61"/>
-      <c r="E313" s="56"/>
-      <c r="F313" s="56"/>
-      <c r="G313" s="57"/>
-      <c r="H313" s="62"/>
+      <c r="C313" s="59" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="D313" s="61" t="n">
+        <v>18.32</v>
+      </c>
+      <c r="E313" s="56" t="n">
+        <v>30.86</v>
+      </c>
+      <c r="F313" s="56" t="n">
+        <v>27.65</v>
+      </c>
+      <c r="G313" s="57" t="n">
+        <v>39.97</v>
+      </c>
+      <c r="H313" s="62" t="n">
+        <v>27.86</v>
+      </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B314" s="157" t="n">
+      <c r="B314" s="143" t="n">
         <v>21</v>
       </c>
-      <c r="C314" s="59"/>
-      <c r="D314" s="61"/>
-      <c r="E314" s="56"/>
-      <c r="F314" s="56"/>
-      <c r="G314" s="57"/>
-      <c r="H314" s="62"/>
+      <c r="C314" s="59" t="n">
+        <v>21.53</v>
+      </c>
+      <c r="D314" s="61" t="n">
+        <v>17.54</v>
+      </c>
+      <c r="E314" s="56" t="n">
+        <v>27.96</v>
+      </c>
+      <c r="F314" s="56" t="n">
+        <v>26.34</v>
+      </c>
+      <c r="G314" s="57" t="n">
+        <v>35.6</v>
+      </c>
+      <c r="H314" s="62" t="n">
+        <v>27.16</v>
+      </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B315" s="157" t="n">
+      <c r="B315" s="143" t="n">
         <v>22</v>
       </c>
-      <c r="C315" s="59"/>
-      <c r="D315" s="61"/>
-      <c r="E315" s="56"/>
-      <c r="F315" s="56"/>
-      <c r="G315" s="57"/>
-      <c r="H315" s="62"/>
+      <c r="C315" s="59" t="n">
+        <v>17.03</v>
+      </c>
+      <c r="D315" s="61" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="E315" s="56" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="F315" s="56" t="n">
+        <v>25.53</v>
+      </c>
+      <c r="G315" s="57" t="n">
+        <v>31.65</v>
+      </c>
+      <c r="H315" s="62" t="n">
+        <v>26.49</v>
+      </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B316" s="157" t="n">
+      <c r="B316" s="143" t="n">
         <v>23</v>
       </c>
-      <c r="C316" s="59"/>
-      <c r="D316" s="61"/>
-      <c r="E316" s="56"/>
-      <c r="F316" s="56"/>
-      <c r="G316" s="57"/>
-      <c r="H316" s="62"/>
+      <c r="C316" s="59" t="n">
+        <v>13.28</v>
+      </c>
+      <c r="D316" s="61" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="E316" s="56" t="n">
+        <v>24.55</v>
+      </c>
+      <c r="F316" s="56" t="n">
+        <v>24.86</v>
+      </c>
+      <c r="G316" s="57" t="n">
+        <v>28.03</v>
+      </c>
+      <c r="H316" s="62" t="n">
+        <v>25.82</v>
+      </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B317" s="158" t="n">
+      <c r="B317" s="144" t="n">
         <v>24</v>
       </c>
-      <c r="C317" s="66"/>
-      <c r="D317" s="69"/>
-      <c r="E317" s="68"/>
-      <c r="F317" s="68"/>
-      <c r="G317" s="86"/>
-      <c r="H317" s="70"/>
+      <c r="C317" s="66" t="n">
+        <v>10.21</v>
+      </c>
+      <c r="D317" s="69" t="n">
+        <v>15.36</v>
+      </c>
+      <c r="E317" s="68" t="n">
+        <v>22.98</v>
+      </c>
+      <c r="F317" s="68" t="n">
+        <v>23.89</v>
+      </c>
+      <c r="G317" s="86" t="n">
+        <v>24.84</v>
+      </c>
+      <c r="H317" s="70" t="n">
+        <v>25.25</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="145"/>

</xml_diff>

<commit_message>
Try tiny change in spreadsheet to trigger recreating files
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484D77F8-E886-4115-A1B8-28A7ADCD765A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F99F5-8DD3-49ED-938C-B555B3786D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="2100" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14325" yWindow="1710" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YourData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="205">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -1160,6 +1160,9 @@
   </si>
   <si>
     <t>Sum (check)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2411,7 @@
   <dimension ref="A3:AO579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C262" sqref="C262"/>
+      <selection activeCell="B255" sqref="B255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7928,7 +7931,9 @@
       <c r="Z254" s="71"/>
     </row>
     <row r="255" spans="2:29" ht="15" x14ac:dyDescent="0.2">
-      <c r="B255" s="144"/>
+      <c r="B255" s="144" t="s">
+        <v>204</v>
+      </c>
       <c r="C255" s="86"/>
       <c r="H255" s="71"/>
       <c r="L255" s="1"/>

</xml_diff>

<commit_message>
Update spreadsheet to trigger refresh of all files
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F99F5-8DD3-49ED-938C-B555B3786D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299DE9D9-B327-4186-9E59-7D769DFBD007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14325" yWindow="1710" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="204">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -1160,9 +1160,6 @@
   </si>
   <si>
     <t>Sum (check)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2411,7 +2408,7 @@
   <dimension ref="A3:AO579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B255" sqref="B255"/>
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7931,9 +7928,7 @@
       <c r="Z254" s="71"/>
     </row>
     <row r="255" spans="2:29" ht="15" x14ac:dyDescent="0.2">
-      <c r="B255" s="144" t="s">
-        <v>204</v>
-      </c>
+      <c r="B255" s="144"/>
       <c r="C255" s="86"/>
       <c r="H255" s="71"/>
       <c r="L255" s="1"/>

</xml_diff>

<commit_message>
Insignificant change to test spreadsheet to prompt updates
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299DE9D9-B327-4186-9E59-7D769DFBD007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2B5B31-54CB-408A-9470-5EF4A60A0BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14325" yWindow="1710" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10020" yWindow="2070" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YourData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="205">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -1160,6 +1160,9 @@
   </si>
   <si>
     <t>Sum (check)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2411,7 @@
   <dimension ref="A3:AO579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+      <selection activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6196,7 +6199,7 @@
       <c r="T208" s="5"/>
       <c r="U208" s="5"/>
     </row>
-    <row r="209" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O209" s="123"/>
       <c r="P209" s="123"/>
       <c r="Q209" s="123"/>
@@ -6205,7 +6208,7 @@
       <c r="T209" s="5"/>
       <c r="U209" s="5"/>
     </row>
-    <row r="210" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O210" s="123"/>
       <c r="P210" s="123"/>
       <c r="Q210" s="123"/>
@@ -6214,7 +6217,7 @@
       <c r="T210" s="5"/>
       <c r="U210" s="5"/>
     </row>
-    <row r="211" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O211" s="123"/>
       <c r="P211" s="123"/>
       <c r="Q211" s="123"/>
@@ -6223,7 +6226,7 @@
       <c r="T211" s="5"/>
       <c r="U211" s="5"/>
     </row>
-    <row r="212" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O212" s="123"/>
       <c r="P212" s="123"/>
       <c r="Q212" s="123"/>
@@ -6232,7 +6235,7 @@
       <c r="T212" s="5"/>
       <c r="U212" s="5"/>
     </row>
-    <row r="213" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O213" s="123"/>
       <c r="P213" s="123"/>
       <c r="Q213" s="123"/>
@@ -6241,7 +6244,7 @@
       <c r="T213" s="5"/>
       <c r="U213" s="5"/>
     </row>
-    <row r="214" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O214" s="123"/>
       <c r="P214" s="123"/>
       <c r="Q214" s="123"/>
@@ -6251,7 +6254,7 @@
       <c r="U214" s="5"/>
       <c r="AB214" s="1"/>
     </row>
-    <row r="215" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O215" s="123"/>
       <c r="P215" s="123"/>
       <c r="Q215" s="123"/>
@@ -6260,7 +6263,7 @@
       <c r="T215" s="5"/>
       <c r="U215" s="5"/>
     </row>
-    <row r="216" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O216" s="123"/>
       <c r="P216" s="123"/>
       <c r="Q216" s="123"/>
@@ -6269,7 +6272,7 @@
       <c r="T216" s="5"/>
       <c r="U216" s="5"/>
     </row>
-    <row r="217" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O217" s="123"/>
       <c r="P217" s="123"/>
       <c r="Q217" s="123"/>
@@ -6278,7 +6281,7 @@
       <c r="T217" s="5"/>
       <c r="U217" s="5"/>
     </row>
-    <row r="218" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O218" s="123"/>
       <c r="P218" s="123"/>
       <c r="Q218" s="123"/>
@@ -6288,7 +6291,7 @@
       <c r="U218" s="5"/>
       <c r="AC218" s="63"/>
     </row>
-    <row r="219" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O219" s="123"/>
       <c r="P219" s="123"/>
       <c r="Q219" s="123"/>
@@ -6298,7 +6301,7 @@
       <c r="U219" s="5"/>
       <c r="AC219" s="63"/>
     </row>
-    <row r="220" spans="15:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="O220" s="123"/>
       <c r="P220" s="123"/>
       <c r="Q220" s="123"/>
@@ -6308,9 +6311,14 @@
       <c r="U220" s="5"/>
       <c r="AC220" s="44"/>
     </row>
-    <row r="221" spans="15:29" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AB221" s="124"/>
       <c r="AC221" s="124"/>
+    </row>
+    <row r="223" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="225" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B225" s="33" t="s">

</xml_diff>

<commit_message>
Change to spreadsheet to trigger github actions
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2B5B31-54CB-408A-9470-5EF4A60A0BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2136CD4-6123-4B88-BF94-33BF5837A707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="2070" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="205">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -2411,7 +2411,7 @@
   <dimension ref="A3:AO579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223"/>
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7944,7 +7944,9 @@
       <c r="Z255" s="71"/>
     </row>
     <row r="256" spans="2:29" ht="15" x14ac:dyDescent="0.2">
-      <c r="B256" s="144"/>
+      <c r="B256" s="144" t="s">
+        <v>204</v>
+      </c>
       <c r="C256" s="86"/>
       <c r="D256" s="125"/>
       <c r="H256" s="71"/>

</xml_diff>

<commit_message>
Update excel file and delete all others to trigger refresh
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2136CD4-6123-4B88-BF94-33BF5837A707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE26ACE1-FB6C-4B16-AFC3-83100C2810C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10020" yWindow="2070" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="205">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -2411,7 +2411,7 @@
   <dimension ref="A3:AO579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6317,6 +6317,9 @@
     </row>
     <row r="223" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
+        <v>204</v>
+      </c>
+      <c r="B223" t="s">
         <v>204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove test 000 results5-2a.json file to try to prompt a refresh and made tiny change to RESULTS5-2A.xlsx
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jglaz\Documents\projects\ANL-Std140-205\automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93244691-1E5A-4203-9CE9-6BC973E1EF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211C217B-9EB9-452E-A3C8-010EAF5828A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="2190" windowWidth="21240" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31425" yWindow="4155" windowWidth="38490" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YourData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="206">
   <si>
     <t xml:space="preserve">STANDARD 140 OUTPUT FORM - RESULTS    </t>
   </si>
@@ -2414,7 +2414,7 @@
   <dimension ref="A3:AO579"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B223" sqref="B223"/>
+      <selection activeCell="B255" sqref="B255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7942,7 +7942,9 @@
       <c r="Z254" s="71"/>
     </row>
     <row r="255" spans="2:29" ht="15" x14ac:dyDescent="0.2">
-      <c r="B255" s="144"/>
+      <c r="B255" s="144" t="s">
+        <v>204</v>
+      </c>
       <c r="C255" s="86"/>
       <c r="H255" s="71"/>
       <c r="L255" s="1"/>

</xml_diff>

<commit_message>
Trying again to prompt full refresh.
</commit_message>
<xml_diff>
--- a/input/Test/0.0.0/RESULTS5-2A.xlsx
+++ b/input/Test/0.0.0/RESULTS5-2A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Test\0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211C217B-9EB9-452E-A3C8-010EAF5828A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8AAA2-7361-4CB7-A59A-7F6381CF4BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31425" yWindow="4155" windowWidth="38490" windowHeight="17445" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7943,7 +7943,7 @@
     </row>
     <row r="255" spans="2:29" ht="15" x14ac:dyDescent="0.2">
       <c r="B255" s="144" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C255" s="86"/>
       <c r="H255" s="71"/>

</xml_diff>